<commit_message>
Finalização das tarefas de documentação -> André Castro
</commit_message>
<xml_diff>
--- a/Documentation/Log.xlsx
+++ b/Documentation/Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>Docs</t>
   </si>
@@ -129,6 +129,27 @@
   </si>
   <si>
     <t>Análise e Espeficicação de Requisitos</t>
+  </si>
+  <si>
+    <t>André Castro</t>
+  </si>
+  <si>
+    <t>[DDet] 3.2.2 - Detalhar o diagrama de classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DDet] 3.2.5 - Diagrama de Navegação </t>
+  </si>
+  <si>
+    <t>[AER] 3.2 - Equipa de desenvolvimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[AER] 3.3 - Ferramentas </t>
+  </si>
+  <si>
+    <t>[AER] 3.4 - Controlo de versões</t>
+  </si>
+  <si>
+    <t>[AER] 7.1.1 – Corrigir os Requisitos Ambientais</t>
   </si>
 </sst>
 </file>
@@ -160,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +206,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -418,36 +445,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -460,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,12 +504,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -523,6 +514,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -532,21 +535,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,12 +1004,12 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.8984375" customWidth="1"/>
@@ -1021,10 +1019,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1053,7 +1051,7 @@
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="11">
@@ -1062,8 +1060,8 @@
       <c r="D3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="31">
-        <v>43655.479166666664</v>
+      <c r="E3" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>16</v>
@@ -1071,7 +1069,7 @@
       <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1079,7 +1077,7 @@
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="12">
@@ -1088,8 +1086,8 @@
       <c r="D4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="32">
-        <v>43655.479166666664</v>
+      <c r="E4" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>17</v>
@@ -1097,13 +1095,13 @@
       <c r="G4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="29"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="12">
@@ -1112,8 +1110,8 @@
       <c r="D5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="32">
-        <v>43655.479166666664</v>
+      <c r="E5" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>18</v>
@@ -1121,13 +1119,13 @@
       <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="29"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="12">
@@ -1136,8 +1134,8 @@
       <c r="D6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="32">
-        <v>43655.479166666664</v>
+      <c r="E6" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>19</v>
@@ -1145,13 +1143,13 @@
       <c r="G6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="29"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="12">
@@ -1160,8 +1158,8 @@
       <c r="D7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="32">
-        <v>43655.479166666664</v>
+      <c r="E7" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>20</v>
@@ -1169,13 +1167,13 @@
       <c r="G7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="29"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="12">
@@ -1184,8 +1182,8 @@
       <c r="D8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="32">
-        <v>43655.479166666664</v>
+      <c r="E8" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>21</v>
@@ -1193,13 +1191,13 @@
       <c r="G8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="12">
@@ -1208,8 +1206,8 @@
       <c r="D9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="32">
-        <v>43655.479166666664</v>
+      <c r="E9" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>22</v>
@@ -1217,13 +1215,13 @@
       <c r="G9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="29"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="12">
@@ -1232,8 +1230,8 @@
       <c r="D10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="32">
-        <v>43655.479166666664</v>
+      <c r="E10" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>23</v>
@@ -1241,43 +1239,47 @@
       <c r="G10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="29"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>2</v>
+      <c r="B11" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="C11" s="12">
-        <v>0</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="33"/>
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="26">
+        <v>43655.666666666664</v>
+      </c>
       <c r="F11" s="18" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="29"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="31"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="12">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="32">
-        <v>43655.5</v>
+      <c r="E12" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>25</v>
@@ -1285,23 +1287,23 @@
       <c r="G12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="29"/>
+      <c r="H12" s="31"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="13">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="34">
-        <v>43655.5</v>
+      <c r="E13" s="26">
+        <v>43655.666666666664</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>26</v>
@@ -1309,7 +1311,7 @@
       <c r="G13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="30"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
@@ -1320,58 +1322,91 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="27">
         <f>SUM(C3:C13)/COUNT(C3:C13)</f>
-        <v>0.74545454545454559</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+        <v>0.86818181818181828</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
     </row>
   </sheetData>
@@ -1380,7 +1415,7 @@
     <mergeCell ref="H3:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C1048576">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1391,16 +1426,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B17 B19:B32">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+  <conditionalFormatting sqref="B3:B17 B19:B24 B31:B32">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C13">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1412,15 +1447,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B25:B30">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:B30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13 B3:B17 B19:B76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13 B3:B17 B19:B24 B31:B76">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>